<commit_message>
Completed video split feature
</commit_message>
<xml_diff>
--- a/docs/VideoSplitterApp_Sch.xlsx
+++ b/docs/VideoSplitterApp_Sch.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="78">
   <si>
     <t>Start Date</t>
   </si>
@@ -144,9 +144,6 @@
     <t>High</t>
   </si>
   <si>
-    <t>Sprint 2 (Associate Profile)</t>
-  </si>
-  <si>
     <t>%Complete</t>
   </si>
   <si>
@@ -253,6 +250,12 @@
   </si>
   <si>
     <t>Github commit</t>
+  </si>
+  <si>
+    <t>Unit Test &amp; Validation</t>
+  </si>
+  <si>
+    <t>Sprint 2 (TBD)</t>
   </si>
 </sst>
 </file>
@@ -261,7 +264,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="m/d;@"/>
+    <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -374,19 +377,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -430,9 +434,9 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -446,7 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -461,11 +465,22 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -529,98 +544,98 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sprint_Schedule!$A$3:$A$50</c:f>
+              <c:f>Sprint_Schedule!$A$12:$A$51</c:f>
               <c:strCache>
-                <c:ptCount val="48"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>Sprint 0 (Set Up &amp; Planning)</c:v>
+                  <c:v>Video Splitter</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Mock Up</c:v>
+                  <c:v>Show select video dialog</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>User Stories</c:v>
+                  <c:v>Show select output folder dialog</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Data Model</c:v>
+                  <c:v>Show processing screen</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Schedule &amp; Planning</c:v>
+                  <c:v>Open output folder</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Sprint 1 (Program Manager Capabilities)</c:v>
+                  <c:v>Unit Test &amp; Validation</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>Video Reassembler</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Prompt for folder to reassemble</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Prompt for reassemble location</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Prompt for frame rate</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Show progress while reassembling</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Save and open reassemble location</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Play in new WPF window</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Unit\Regression Testing</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Usability testing\Deployment\Security Review\Refactoring</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Milestone 1 (Able to split video, Able to reassemble video)</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Sprint 2 (TBD)</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>Sprint Planning</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="18">
                   <c:v>Requirements Specification</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="19">
                   <c:v>Architecture\Design</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>Video Splitter</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Show select video dialog</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Show select output folder dialog</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Show processing screen</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Open output folder</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Video Reassembler</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Prompt for folder to reassemble</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Prompt for reassemble location</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Prompt for frame rate</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Show progress while reassembling</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Save and open reassemble location</c:v>
-                </c:pt>
                 <c:pt idx="20">
-                  <c:v>Play in new WPF window</c:v>
+                  <c:v>Profile Manager</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>View Profile</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>Unit\Regression Testing</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>Usability testing\Deployment\Security Review\Refactoring</c:v>
                 </c:pt>
-                <c:pt idx="23">
-                  <c:v>Milestone 1 (Able to split video, Able to reassemble video)</c:v>
-                </c:pt>
                 <c:pt idx="24">
-                  <c:v>Sprint 2 (Associate Profile)</c:v>
+                  <c:v>Milestone 1 ( Demo Program Manager, Associate Profile Capabilities)</c:v>
                 </c:pt>
                 <c:pt idx="25">
+                  <c:v>Sprint 3 (TBD)</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>Sprint Planning</c:v>
                 </c:pt>
-                <c:pt idx="26">
-                  <c:v>Requirements Specification</c:v>
-                </c:pt>
                 <c:pt idx="27">
+                  <c:v>Requirements Specification </c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>Architecture\Design</c:v>
                 </c:pt>
-                <c:pt idx="28">
-                  <c:v>Profile Manager</c:v>
-                </c:pt>
                 <c:pt idx="29">
-                  <c:v>View Profile</c:v>
+                  <c:v>Feature Development</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>Unit\Regression Testing</c:v>
@@ -629,51 +644,27 @@
                   <c:v>Usability testing\Deployment\Security Review\Refactoring</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>Milestone 1 ( Demo Program Manager, Associate Profile Capabilities)</c:v>
+                  <c:v>Sprint 4 (TBD)</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>Sprint 3 (TBD)</c:v>
+                  <c:v>Sprint Planning</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>Sprint Planning</c:v>
+                  <c:v>Requirements Specification </c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>Requirements Specification </c:v>
+                  <c:v>Architecture\Design</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>Architecture\Design</c:v>
+                  <c:v>Feature Development</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>Feature Development</c:v>
+                  <c:v>Unit\Regression Testing</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>Unit\Regression Testing</c:v>
+                  <c:v>Usability testing\Deployment\Security Review\Refactoring</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>Usability testing\Deployment\Security Review\Refactoring</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>Sprint 4 (TBD)</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>Sprint Planning</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>Requirements Specification </c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>Architecture\Design</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>Feature Development</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>Unit\Regression Testing</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>Usability testing\Deployment\Security Review\Refactoring</c:v>
-                </c:pt>
-                <c:pt idx="47">
                   <c:v>Milestone 2 (TBD)</c:v>
                 </c:pt>
               </c:strCache>
@@ -681,153 +672,129 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sprint_Schedule!$B$3:$B$50</c:f>
+              <c:f>Sprint_Schedule!$B$12:$B$51</c:f>
               <c:numCache>
                 <c:formatCode>m/d;@</c:formatCode>
-                <c:ptCount val="48"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>41493</c:v>
+                  <c:v>41494</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41493</c:v>
+                  <c:v>41546</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41493</c:v>
+                  <c:v>41546</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41493</c:v>
+                  <c:v>41546</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41493</c:v>
+                  <c:v>41546</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41494</c:v>
+                  <c:v>41547</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41494</c:v>
+                  <c:v>41547</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41494</c:v>
+                  <c:v>41547</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41494</c:v>
+                  <c:v>41547</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41494</c:v>
+                  <c:v>41547</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41494</c:v>
+                  <c:v>41547</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>41494</c:v>
+                  <c:v>41547</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41494</c:v>
+                  <c:v>41547</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>41494</c:v>
+                  <c:v>41547</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>41494</c:v>
+                  <c:v>41547</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>41494</c:v>
+                  <c:v>41547</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41494</c:v>
+                  <c:v>41548</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41494</c:v>
+                  <c:v>41548</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>41494</c:v>
+                  <c:v>41548</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41494</c:v>
+                  <c:v>41548</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41494</c:v>
+                  <c:v>41548</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41494</c:v>
+                  <c:v>41548</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>41494</c:v>
+                  <c:v>41548</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>41494</c:v>
+                  <c:v>41548</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>41495</c:v>
+                  <c:v>41548</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41495</c:v>
+                  <c:v>41549</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41495</c:v>
+                  <c:v>41549</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>41495</c:v>
+                  <c:v>41549</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>41495</c:v>
+                  <c:v>41549</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>41495</c:v>
+                  <c:v>41549</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>41495</c:v>
+                  <c:v>41549</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>41495</c:v>
+                  <c:v>41549</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>41495</c:v>
+                  <c:v>41550</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>41496</c:v>
+                  <c:v>41550</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>41496</c:v>
+                  <c:v>41550</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>41496</c:v>
+                  <c:v>41550</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>41496</c:v>
+                  <c:v>41550</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>41496</c:v>
+                  <c:v>41550</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>41496</c:v>
+                  <c:v>41550</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>41496</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>41497</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>41497</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>41497</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>41497</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>41497</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>41497</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>41497</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>41497</c:v>
+                  <c:v>41550</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -859,7 +826,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -902,7 +869,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
+                <a:srgbClr val="00FF00"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1101,98 +1068,98 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Sprint_Schedule!$A$3:$A$50</c:f>
+              <c:f>Sprint_Schedule!$A$12:$A$51</c:f>
               <c:strCache>
-                <c:ptCount val="48"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>Sprint 0 (Set Up &amp; Planning)</c:v>
+                  <c:v>Video Splitter</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Mock Up</c:v>
+                  <c:v>Show select video dialog</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>User Stories</c:v>
+                  <c:v>Show select output folder dialog</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Data Model</c:v>
+                  <c:v>Show processing screen</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Schedule &amp; Planning</c:v>
+                  <c:v>Open output folder</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Sprint 1 (Program Manager Capabilities)</c:v>
+                  <c:v>Unit Test &amp; Validation</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>Video Reassembler</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Prompt for folder to reassemble</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Prompt for reassemble location</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Prompt for frame rate</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Show progress while reassembling</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Save and open reassemble location</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Play in new WPF window</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Unit\Regression Testing</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Usability testing\Deployment\Security Review\Refactoring</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Milestone 1 (Able to split video, Able to reassemble video)</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Sprint 2 (TBD)</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>Sprint Planning</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="18">
                   <c:v>Requirements Specification</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="19">
                   <c:v>Architecture\Design</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>Video Splitter</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Show select video dialog</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Show select output folder dialog</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Show processing screen</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Open output folder</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Video Reassembler</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Prompt for folder to reassemble</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Prompt for reassemble location</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Prompt for frame rate</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Show progress while reassembling</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Save and open reassemble location</c:v>
-                </c:pt>
                 <c:pt idx="20">
-                  <c:v>Play in new WPF window</c:v>
+                  <c:v>Profile Manager</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>View Profile</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>Unit\Regression Testing</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>Usability testing\Deployment\Security Review\Refactoring</c:v>
                 </c:pt>
-                <c:pt idx="23">
-                  <c:v>Milestone 1 (Able to split video, Able to reassemble video)</c:v>
-                </c:pt>
                 <c:pt idx="24">
-                  <c:v>Sprint 2 (Associate Profile)</c:v>
+                  <c:v>Milestone 1 ( Demo Program Manager, Associate Profile Capabilities)</c:v>
                 </c:pt>
                 <c:pt idx="25">
+                  <c:v>Sprint 3 (TBD)</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>Sprint Planning</c:v>
                 </c:pt>
-                <c:pt idx="26">
-                  <c:v>Requirements Specification</c:v>
-                </c:pt>
                 <c:pt idx="27">
+                  <c:v>Requirements Specification </c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>Architecture\Design</c:v>
                 </c:pt>
-                <c:pt idx="28">
-                  <c:v>Profile Manager</c:v>
-                </c:pt>
                 <c:pt idx="29">
-                  <c:v>View Profile</c:v>
+                  <c:v>Feature Development</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>Unit\Regression Testing</c:v>
@@ -1201,51 +1168,27 @@
                   <c:v>Usability testing\Deployment\Security Review\Refactoring</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>Milestone 1 ( Demo Program Manager, Associate Profile Capabilities)</c:v>
+                  <c:v>Sprint 4 (TBD)</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>Sprint 3 (TBD)</c:v>
+                  <c:v>Sprint Planning</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>Sprint Planning</c:v>
+                  <c:v>Requirements Specification </c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>Requirements Specification </c:v>
+                  <c:v>Architecture\Design</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>Architecture\Design</c:v>
+                  <c:v>Feature Development</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>Feature Development</c:v>
+                  <c:v>Unit\Regression Testing</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>Unit\Regression Testing</c:v>
+                  <c:v>Usability testing\Deployment\Security Review\Refactoring</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>Usability testing\Deployment\Security Review\Refactoring</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>Sprint 4 (TBD)</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>Sprint Planning</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>Requirements Specification </c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>Architecture\Design</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>Feature Development</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>Unit\Regression Testing</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>Usability testing\Deployment\Security Review\Refactoring</c:v>
-                </c:pt>
-                <c:pt idx="47">
                   <c:v>Milestone 2 (TBD)</c:v>
                 </c:pt>
               </c:strCache>
@@ -1253,21 +1196,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sprint_Schedule!$C$3:$C$50</c:f>
+              <c:f>Sprint_Schedule!$C$12:$C$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="48"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -1375,30 +1318,6 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="47">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1415,11 +1334,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="402243208"/>
-        <c:axId val="402246736"/>
+        <c:axId val="302140064"/>
+        <c:axId val="302141632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="402243208"/>
+        <c:axId val="302140064"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1446,7 +1365,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="402246736"/>
+        <c:crossAx val="302141632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1454,11 +1373,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="402246736"/>
+        <c:axId val="302141632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="41513"/>
-          <c:min val="41490"/>
+          <c:max val="41573"/>
+          <c:min val="41545"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -1484,7 +1403,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="402243208"/>
+        <c:crossAx val="302140064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2"/>
@@ -1533,7 +1452,7 @@
     <xdr:to>
       <xdr:col>31</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1562,12 +1481,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.38116</cdr:x>
-      <cdr:y>0.13086</cdr:y>
+      <cdr:x>0.31061</cdr:x>
+      <cdr:y>0.14661</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.38767</cdr:x>
-      <cdr:y>0.35087</cdr:y>
+      <cdr:x>0.31712</cdr:x>
+      <cdr:y>0.36662</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -1576,8 +1495,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="16200000">
-          <a:off x="4985563" y="2668238"/>
-          <a:ext cx="2485376" cy="105450"/>
+          <a:off x="3821659" y="2895089"/>
+          <a:ext cx="2527288" cy="105475"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rightArrow">
           <a:avLst/>
@@ -1719,12 +1638,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.38582</cdr:x>
-      <cdr:y>0.08545</cdr:y>
+      <cdr:x>0.32879</cdr:x>
+      <cdr:y>0.13271</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.55133</cdr:x>
-      <cdr:y>0.09411</cdr:y>
+      <cdr:x>0.4943</cdr:x>
+      <cdr:y>0.14137</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -1733,8 +1652,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="10800000" flipV="1">
-          <a:off x="6251135" y="965335"/>
-          <a:ext cx="2681581" cy="97801"/>
+          <a:off x="5327140" y="1524502"/>
+          <a:ext cx="2681597" cy="99479"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rightArrow">
           <a:avLst/>
@@ -2166,10 +2085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2192,7 +2111,7 @@
         <v>10</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>4</v>
@@ -2281,14 +2200,14 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>6</v>
+        <v>49</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>5</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>11</v>
@@ -2300,13 +2219,13 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>6</v>
+        <v>49</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>28</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>11</v>
@@ -2314,13 +2233,13 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>6</v>
+        <v>49</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>28</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>11</v>
@@ -2328,13 +2247,13 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>6</v>
+        <v>49</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>28</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>11</v>
@@ -2342,24 +2261,24 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>6</v>
+        <v>49</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>28</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>47</v>
+      <c r="A11" s="40" t="s">
+        <v>76</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D11" s="25" t="s">
         <v>6</v>
@@ -2369,11 +2288,11 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
-        <v>57</v>
+      <c r="A12" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="25" t="s">
         <v>6</v>
@@ -2384,10 +2303,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D13" s="25" t="s">
         <v>6</v>
@@ -2398,10 +2317,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="25" t="s">
         <v>6</v>
@@ -2412,10 +2331,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" s="25" t="s">
         <v>6</v>
@@ -2426,11 +2345,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="1"/>
+        <v>59</v>
+      </c>
       <c r="C16" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" s="25" t="s">
         <v>6</v>
@@ -2440,12 +2358,12 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>48</v>
+      <c r="A17" s="16" t="s">
+        <v>60</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D17" s="25" t="s">
         <v>6</v>
@@ -2455,11 +2373,12 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="40" t="s">
-        <v>62</v>
-      </c>
+      <c r="A18" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="1"/>
       <c r="C18" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D18" s="25" t="s">
         <v>6</v>
@@ -2470,10 +2389,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" s="25" t="s">
         <v>6</v>
@@ -2484,10 +2403,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="40" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D20" s="25" t="s">
         <v>6</v>
@@ -2498,10 +2417,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="40" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" s="25" t="s">
         <v>6</v>
@@ -2512,10 +2431,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="40" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D22" s="25" t="s">
         <v>6</v>
@@ -2526,16 +2445,35 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="40" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" s="25" t="s">
         <v>6</v>
       </c>
       <c r="E23" s="17" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="36" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2549,15 +2487,16 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="97.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.7109375" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" style="21" customWidth="1"/>
-    <col min="4" max="5" width="14.7109375" style="17" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="17" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="43" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" style="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" style="10" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" style="21" customWidth="1"/>
@@ -2576,8 +2515,8 @@
       <c r="D1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>41</v>
+      <c r="E1" s="41" t="s">
+        <v>40</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>17</v>
@@ -2600,12 +2539,12 @@
     </row>
     <row r="2" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="E2" s="42"/>
       <c r="F2" s="20"/>
       <c r="G2" s="30"/>
       <c r="H2" s="20"/>
@@ -2615,15 +2554,17 @@
         <v>13</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>6</v>
+        <v>42</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>5</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="17"/>
+      <c r="E3" s="43">
+        <v>0.9</v>
+      </c>
       <c r="F3" s="21"/>
       <c r="G3" s="10"/>
       <c r="H3" s="21"/>
@@ -2633,7 +2574,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>6</v>
@@ -2641,7 +2582,9 @@
       <c r="D4" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="17"/>
+      <c r="E4" s="43">
+        <v>0</v>
+      </c>
       <c r="F4" s="21"/>
       <c r="G4" s="10"/>
       <c r="H4" s="21"/>
@@ -2651,7 +2594,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>6</v>
@@ -2659,14 +2602,16 @@
       <c r="D5" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="17"/>
+      <c r="E5" s="43">
+        <v>0</v>
+      </c>
       <c r="F5" s="21"/>
       <c r="G5" s="10"/>
       <c r="H5" s="21"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2677,10 +2622,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2735,7 +2680,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="26">
-        <f t="shared" ref="D3:D23" si="0">B3+C3</f>
+        <f t="shared" ref="D3:D24" si="0">B3+C3</f>
         <v>41494</v>
       </c>
       <c r="E3" s="24" t="s">
@@ -2744,7 +2689,7 @@
     </row>
     <row r="4" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="6">
         <v>41493</v>
@@ -2762,7 +2707,7 @@
     </row>
     <row r="5" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="6">
         <v>41493</v>
@@ -2780,7 +2725,7 @@
     </row>
     <row r="6" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="6">
         <v>41493</v>
@@ -2798,7 +2743,7 @@
     </row>
     <row r="7" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" s="6">
         <v>41493</v>
@@ -2844,8 +2789,8 @@
         <f t="shared" si="0"/>
         <v>41495</v>
       </c>
-      <c r="E9" s="25" t="s">
-        <v>6</v>
+      <c r="E9" s="23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2862,8 +2807,8 @@
         <f t="shared" si="0"/>
         <v>41495</v>
       </c>
-      <c r="E10" s="25" t="s">
-        <v>6</v>
+      <c r="E10" s="23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2880,13 +2825,13 @@
         <f t="shared" si="0"/>
         <v>41495</v>
       </c>
-      <c r="E11" s="25" t="s">
-        <v>6</v>
+      <c r="E11" s="23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="6">
         <v>41494</v>
@@ -2898,113 +2843,113 @@
         <f t="shared" si="0"/>
         <v>41495</v>
       </c>
-      <c r="E12" s="25" t="s">
-        <v>6</v>
+      <c r="E12" s="23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" s="6">
-        <v>41494</v>
+        <v>41546</v>
       </c>
       <c r="C13" s="15">
         <v>1</v>
       </c>
       <c r="D13" s="6">
         <f t="shared" si="0"/>
-        <v>41495</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>6</v>
+        <v>41547</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14" s="6">
-        <v>41494</v>
+        <v>41546</v>
       </c>
       <c r="C14" s="15">
         <v>1</v>
       </c>
       <c r="D14" s="6">
         <f t="shared" si="0"/>
-        <v>41495</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>6</v>
+        <v>41547</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" s="6">
-        <v>41494</v>
+        <v>41546</v>
       </c>
       <c r="C15" s="15">
         <v>1</v>
       </c>
       <c r="D15" s="6">
         <f t="shared" si="0"/>
-        <v>41495</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>6</v>
+        <v>41547</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="6">
-        <v>41494</v>
+        <v>41546</v>
       </c>
       <c r="C16" s="15">
         <v>1</v>
       </c>
       <c r="D16" s="6">
         <f t="shared" si="0"/>
-        <v>41495</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>6</v>
+        <v>41547</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>48</v>
+      <c r="A17" s="40" t="s">
+        <v>76</v>
       </c>
       <c r="B17" s="6">
-        <v>41494</v>
+        <v>41547</v>
       </c>
       <c r="C17" s="15">
         <v>1</v>
       </c>
       <c r="D17" s="6">
-        <f t="shared" si="0"/>
-        <v>41495</v>
+        <f t="shared" ref="D17" si="1">B17+C17</f>
+        <v>41548</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="40" t="s">
-        <v>62</v>
+      <c r="A18" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="B18" s="6">
-        <v>41494</v>
+        <v>41547</v>
       </c>
       <c r="C18" s="15">
         <v>1</v>
       </c>
       <c r="D18" s="6">
         <f t="shared" si="0"/>
-        <v>41495</v>
+        <v>41548</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>6</v>
@@ -3012,17 +2957,17 @@
     </row>
     <row r="19" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B19" s="6">
-        <v>41494</v>
+        <v>41547</v>
       </c>
       <c r="C19" s="15">
         <v>1</v>
       </c>
       <c r="D19" s="6">
         <f t="shared" si="0"/>
-        <v>41495</v>
+        <v>41548</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>6</v>
@@ -3030,17 +2975,17 @@
     </row>
     <row r="20" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="40" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B20" s="6">
-        <v>41494</v>
+        <v>41547</v>
       </c>
       <c r="C20" s="15">
         <v>1</v>
       </c>
       <c r="D20" s="6">
         <f t="shared" si="0"/>
-        <v>41495</v>
+        <v>41548</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>6</v>
@@ -3048,17 +2993,17 @@
     </row>
     <row r="21" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B21" s="6">
-        <v>41494</v>
+        <v>41547</v>
       </c>
       <c r="C21" s="15">
         <v>1</v>
       </c>
       <c r="D21" s="6">
         <f t="shared" si="0"/>
-        <v>41495</v>
+        <v>41548</v>
       </c>
       <c r="E21" s="25" t="s">
         <v>6</v>
@@ -3066,17 +3011,17 @@
     </row>
     <row r="22" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="40" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B22" s="6">
-        <v>41494</v>
+        <v>41547</v>
       </c>
       <c r="C22" s="15">
         <v>1</v>
       </c>
       <c r="D22" s="6">
         <f t="shared" si="0"/>
-        <v>41495</v>
+        <v>41548</v>
       </c>
       <c r="E22" s="25" t="s">
         <v>6</v>
@@ -3084,35 +3029,35 @@
     </row>
     <row r="23" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="40" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B23" s="6">
-        <v>41494</v>
+        <v>41547</v>
       </c>
       <c r="C23" s="15">
         <v>1</v>
       </c>
       <c r="D23" s="6">
         <f t="shared" si="0"/>
-        <v>41495</v>
+        <v>41548</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>8</v>
+      <c r="A24" s="40" t="s">
+        <v>66</v>
       </c>
       <c r="B24" s="6">
-        <v>41494</v>
+        <v>41547</v>
       </c>
       <c r="C24" s="15">
         <v>1</v>
       </c>
       <c r="D24" s="6">
-        <f t="shared" ref="D24:D26" si="1">B24+C24</f>
-        <v>41495</v>
+        <f t="shared" si="0"/>
+        <v>41548</v>
       </c>
       <c r="E24" s="25" t="s">
         <v>6</v>
@@ -3120,87 +3065,87 @@
     </row>
     <row r="25" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="6">
+        <v>41547</v>
+      </c>
+      <c r="C25" s="15">
+        <v>1</v>
+      </c>
+      <c r="D25" s="6">
+        <f t="shared" ref="D25:D27" si="2">B25+C25</f>
+        <v>41548</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="6">
-        <v>41494</v>
-      </c>
-      <c r="C25" s="15">
-        <v>1</v>
-      </c>
-      <c r="D25" s="6">
-        <f t="shared" si="1"/>
-        <v>41495</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" s="28">
-        <v>41494</v>
-      </c>
-      <c r="C26" s="27">
-        <v>1</v>
-      </c>
-      <c r="D26" s="28">
-        <f t="shared" si="1"/>
-        <v>41495</v>
+      <c r="B26" s="6">
+        <v>41547</v>
+      </c>
+      <c r="C26" s="15">
+        <v>1</v>
+      </c>
+      <c r="D26" s="6">
+        <f t="shared" si="2"/>
+        <v>41548</v>
       </c>
       <c r="E26" s="25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="26">
-        <v>41495</v>
-      </c>
-      <c r="C27" s="3">
-        <v>1</v>
-      </c>
-      <c r="D27" s="26">
-        <f t="shared" ref="D27:D32" si="2">B27+C27</f>
-        <v>41496</v>
-      </c>
-      <c r="E27" s="26"/>
+    <row r="27" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="28">
+        <v>41547</v>
+      </c>
+      <c r="C27" s="27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="28">
+        <f t="shared" si="2"/>
+        <v>41548</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="28" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="6">
-        <v>41495</v>
-      </c>
-      <c r="C28" s="15">
-        <v>1</v>
-      </c>
-      <c r="D28" s="6">
-        <f t="shared" si="2"/>
-        <v>41496</v>
-      </c>
-      <c r="E28" s="25" t="s">
-        <v>6</v>
-      </c>
+      <c r="A28" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="26">
+        <v>41548</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1</v>
+      </c>
+      <c r="D28" s="26">
+        <f t="shared" ref="D28:D33" si="3">B28+C28</f>
+        <v>41549</v>
+      </c>
+      <c r="E28" s="26"/>
     </row>
     <row r="29" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B29" s="6">
-        <v>41495</v>
+        <v>41548</v>
       </c>
       <c r="C29" s="15">
         <v>1</v>
       </c>
       <c r="D29" s="6">
-        <f t="shared" si="2"/>
-        <v>41496</v>
+        <f t="shared" si="3"/>
+        <v>41549</v>
       </c>
       <c r="E29" s="25" t="s">
         <v>6</v>
@@ -3208,71 +3153,71 @@
     </row>
     <row r="30" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6">
+        <v>41548</v>
+      </c>
+      <c r="C30" s="15">
+        <v>1</v>
+      </c>
+      <c r="D30" s="6">
+        <f t="shared" si="3"/>
+        <v>41549</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="6">
-        <v>41495</v>
-      </c>
-      <c r="C30" s="15">
-        <v>1</v>
-      </c>
-      <c r="D30" s="6">
-        <f t="shared" si="2"/>
-        <v>41496</v>
-      </c>
-      <c r="E30" s="25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
+      <c r="B31" s="6">
+        <v>41548</v>
+      </c>
+      <c r="C31" s="15">
+        <v>1</v>
+      </c>
+      <c r="D31" s="6">
+        <f t="shared" si="3"/>
+        <v>41549</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="6">
-        <v>41495</v>
-      </c>
-      <c r="C31" s="15">
-        <v>1</v>
-      </c>
-      <c r="D31" s="6">
-        <f t="shared" si="2"/>
-        <v>41496</v>
-      </c>
-      <c r="E31" s="25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="33" t="s">
+      <c r="B32" s="6">
+        <v>41548</v>
+      </c>
+      <c r="C32" s="15">
+        <v>1</v>
+      </c>
+      <c r="D32" s="6">
+        <f t="shared" si="3"/>
+        <v>41549</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="6">
-        <v>41495</v>
-      </c>
-      <c r="C32" s="15">
-        <v>1</v>
-      </c>
-      <c r="D32" s="34">
-        <f t="shared" si="2"/>
-        <v>41496</v>
-      </c>
-      <c r="E32" s="25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="B33" s="6">
-        <v>41495</v>
+        <v>41548</v>
       </c>
       <c r="C33" s="15">
         <v>1</v>
       </c>
-      <c r="D33" s="6">
-        <f t="shared" ref="D33:D47" si="3">B33+C33</f>
-        <v>41496</v>
+      <c r="D33" s="34">
+        <f t="shared" si="3"/>
+        <v>41549</v>
       </c>
       <c r="E33" s="25" t="s">
         <v>6</v>
@@ -3280,87 +3225,87 @@
     </row>
     <row r="34" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="6">
+        <v>41548</v>
+      </c>
+      <c r="C34" s="15">
+        <v>1</v>
+      </c>
+      <c r="D34" s="6">
+        <f t="shared" ref="D34:D48" si="4">B34+C34</f>
+        <v>41549</v>
+      </c>
+      <c r="E34" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="6">
-        <v>41495</v>
-      </c>
-      <c r="C34" s="15">
-        <v>1</v>
-      </c>
-      <c r="D34" s="6">
-        <f t="shared" si="3"/>
-        <v>41496</v>
-      </c>
-      <c r="E34" s="25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="27" t="s">
+      <c r="B35" s="6">
+        <v>41548</v>
+      </c>
+      <c r="C35" s="15">
+        <v>1</v>
+      </c>
+      <c r="D35" s="6">
+        <f t="shared" si="4"/>
+        <v>41549</v>
+      </c>
+      <c r="E35" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="28">
-        <v>41495</v>
-      </c>
-      <c r="C35" s="27">
-        <v>1</v>
-      </c>
-      <c r="D35" s="28">
-        <f t="shared" si="3"/>
-        <v>41496</v>
-      </c>
-      <c r="E35" s="25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="B36" s="28">
+        <v>41548</v>
+      </c>
+      <c r="C36" s="27">
+        <v>1</v>
+      </c>
+      <c r="D36" s="28">
+        <f t="shared" si="4"/>
+        <v>41549</v>
+      </c>
+      <c r="E36" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="26">
-        <v>41496</v>
-      </c>
-      <c r="C36" s="3">
-        <v>1</v>
-      </c>
-      <c r="D36" s="26">
-        <f t="shared" ref="D36:D42" si="4">B36+C36</f>
-        <v>41497</v>
-      </c>
-      <c r="E36" s="9"/>
-    </row>
-    <row r="37" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B37" s="6">
-        <v>41496</v>
-      </c>
-      <c r="C37" s="15">
-        <v>1</v>
-      </c>
-      <c r="D37" s="6">
-        <f t="shared" si="4"/>
-        <v>41497</v>
-      </c>
-      <c r="E37" s="25" t="s">
-        <v>6</v>
-      </c>
+      <c r="B37" s="26">
+        <v>41549</v>
+      </c>
+      <c r="C37" s="3">
+        <v>1</v>
+      </c>
+      <c r="D37" s="26">
+        <f t="shared" ref="D37:D43" si="5">B37+C37</f>
+        <v>41550</v>
+      </c>
+      <c r="E37" s="9"/>
     </row>
     <row r="38" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B38" s="6">
-        <v>41496</v>
+        <v>22</v>
+      </c>
+      <c r="B38" s="44">
+        <v>41549</v>
       </c>
       <c r="C38" s="15">
         <v>1</v>
       </c>
       <c r="D38" s="6">
-        <f t="shared" si="4"/>
-        <v>41497</v>
+        <f t="shared" si="5"/>
+        <v>41550</v>
       </c>
       <c r="E38" s="25" t="s">
         <v>6</v>
@@ -3368,53 +3313,53 @@
     </row>
     <row r="39" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" s="6">
+        <v>41549</v>
+      </c>
+      <c r="C39" s="15">
+        <v>1</v>
+      </c>
+      <c r="D39" s="6">
+        <f t="shared" si="5"/>
+        <v>41550</v>
+      </c>
+      <c r="E39" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="6">
-        <v>41496</v>
-      </c>
-      <c r="C39" s="15">
-        <v>1</v>
-      </c>
-      <c r="D39" s="6">
-        <f t="shared" si="4"/>
-        <v>41497</v>
-      </c>
-      <c r="E39" s="25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="15" t="s">
+      <c r="B40" s="6">
+        <v>41549</v>
+      </c>
+      <c r="C40" s="15">
+        <v>1</v>
+      </c>
+      <c r="D40" s="6">
+        <f t="shared" si="5"/>
+        <v>41550</v>
+      </c>
+      <c r="E40" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="6">
-        <v>41496</v>
-      </c>
-      <c r="C40" s="15">
-        <v>1</v>
-      </c>
-      <c r="D40" s="6">
-        <f t="shared" si="4"/>
-        <v>41497</v>
-      </c>
-      <c r="E40" s="25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="B41" s="6">
-        <v>41496</v>
+        <v>41549</v>
       </c>
       <c r="C41" s="15">
         <v>1</v>
       </c>
       <c r="D41" s="6">
-        <f t="shared" si="4"/>
-        <v>41497</v>
+        <f t="shared" si="5"/>
+        <v>41550</v>
       </c>
       <c r="E41" s="25" t="s">
         <v>6</v>
@@ -3422,69 +3367,69 @@
     </row>
     <row r="42" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="6">
+        <v>41549</v>
+      </c>
+      <c r="C42" s="15">
+        <v>1</v>
+      </c>
+      <c r="D42" s="6">
+        <f t="shared" si="5"/>
+        <v>41550</v>
+      </c>
+      <c r="E42" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="6">
-        <v>41496</v>
-      </c>
-      <c r="C42" s="15">
-        <v>1</v>
-      </c>
-      <c r="D42" s="6">
+      <c r="B43" s="6">
+        <v>41549</v>
+      </c>
+      <c r="C43" s="15">
+        <v>1</v>
+      </c>
+      <c r="D43" s="6">
+        <f t="shared" si="5"/>
+        <v>41550</v>
+      </c>
+      <c r="E43" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="26">
+        <v>41550</v>
+      </c>
+      <c r="C44" s="3">
+        <v>1</v>
+      </c>
+      <c r="D44" s="26">
         <f t="shared" si="4"/>
-        <v>41497</v>
-      </c>
-      <c r="E42" s="25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B43" s="26">
-        <v>41497</v>
-      </c>
-      <c r="C43" s="3">
-        <v>1</v>
-      </c>
-      <c r="D43" s="26">
-        <f t="shared" si="3"/>
-        <v>41498</v>
-      </c>
-      <c r="E43" s="9"/>
-    </row>
-    <row r="44" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B44" s="6">
-        <v>41497</v>
-      </c>
-      <c r="C44" s="7">
-        <v>1</v>
-      </c>
-      <c r="D44" s="6">
-        <f t="shared" si="3"/>
-        <v>41498</v>
-      </c>
-      <c r="E44" s="25" t="s">
-        <v>6</v>
-      </c>
+        <v>41551</v>
+      </c>
+      <c r="E44" s="9"/>
     </row>
     <row r="45" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B45" s="6">
-        <v>41497</v>
+        <v>41550</v>
       </c>
       <c r="C45" s="7">
         <v>1</v>
       </c>
       <c r="D45" s="6">
-        <f t="shared" si="3"/>
-        <v>41498</v>
+        <f t="shared" si="4"/>
+        <v>41551</v>
       </c>
       <c r="E45" s="25" t="s">
         <v>6</v>
@@ -3492,53 +3437,53 @@
     </row>
     <row r="46" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" s="6">
+        <v>41550</v>
+      </c>
+      <c r="C46" s="7">
+        <v>1</v>
+      </c>
+      <c r="D46" s="6">
+        <f t="shared" si="4"/>
+        <v>41551</v>
+      </c>
+      <c r="E46" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B46" s="6">
-        <v>41497</v>
-      </c>
-      <c r="C46" s="7">
-        <v>1</v>
-      </c>
-      <c r="D46" s="6">
-        <f t="shared" si="3"/>
-        <v>41498</v>
-      </c>
-      <c r="E46" s="25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
+      <c r="B47" s="6">
+        <v>41550</v>
+      </c>
+      <c r="C47" s="7">
+        <v>1</v>
+      </c>
+      <c r="D47" s="6">
+        <f t="shared" si="4"/>
+        <v>41551</v>
+      </c>
+      <c r="E47" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B47" s="6">
-        <v>41497</v>
-      </c>
-      <c r="C47" s="7">
-        <v>1</v>
-      </c>
-      <c r="D47" s="6">
-        <f t="shared" si="3"/>
-        <v>41498</v>
-      </c>
-      <c r="E47" s="25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="B48" s="6">
-        <v>41497</v>
+        <v>41550</v>
       </c>
       <c r="C48" s="7">
         <v>1</v>
       </c>
       <c r="D48" s="6">
-        <f>B48+C48</f>
-        <v>41498</v>
+        <f t="shared" si="4"/>
+        <v>41551</v>
       </c>
       <c r="E48" s="25" t="s">
         <v>6</v>
@@ -3546,45 +3491,63 @@
     </row>
     <row r="49" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B49" s="6">
-        <v>41497</v>
+        <v>41550</v>
       </c>
       <c r="C49" s="7">
         <v>1</v>
       </c>
       <c r="D49" s="6">
         <f>B49+C49</f>
-        <v>41498</v>
+        <v>41551</v>
       </c>
       <c r="E49" s="25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="27" t="s">
+    <row r="50" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50" s="6">
+        <v>41550</v>
+      </c>
+      <c r="C50" s="7">
+        <v>1</v>
+      </c>
+      <c r="D50" s="6">
+        <f>B50+C50</f>
+        <v>41551</v>
+      </c>
+      <c r="E50" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="28">
-        <v>41497</v>
-      </c>
-      <c r="C50" s="27">
-        <v>1</v>
-      </c>
-      <c r="D50" s="28">
-        <f>B50+C50</f>
-        <v>41498</v>
-      </c>
-      <c r="E50" s="25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="1"/>
+      <c r="B51" s="28">
+        <v>41550</v>
+      </c>
+      <c r="C51" s="27">
+        <v>1</v>
+      </c>
+      <c r="D51" s="28">
+        <f>B51+C51</f>
+        <v>41551</v>
+      </c>
+      <c r="E51" s="25" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3610,17 +3573,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -3641,6 +3604,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BD2D3C48E37A8948BB604D1D3AEC5713" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="be84b0a4d485c09a5a25e1644380b8db">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -3689,12 +3658,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{484E01B0-F78A-4E90-8A17-7A0831AB2514}">
   <ds:schemaRefs>
@@ -3704,6 +3667,20 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CFACB7F-ED1A-4B2F-B06A-9306C6409F1F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3F0FDC7-E0C2-41A3-85B3-61341D152865}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3716,18 +3693,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CFACB7F-ED1A-4B2F-B06A-9306C6409F1F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>